<commit_message>
Actualizacion datos y notebook
</commit_message>
<xml_diff>
--- a/menor_trafico.xlsx
+++ b/menor_trafico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mi unidad\Esp. Big Data\Gestión y almacenamiento de datos\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{941379C0-7449-47E0-B0DA-509D636A96EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCE7475-6EE4-4B69-B144-A8E73BF512EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B6FFDE54-CDE2-4DFD-9040-A33C07424636}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,13 +450,13 @@
         <v>0.25</v>
       </c>
       <c r="B2">
-        <v>239</v>
+        <v>110</v>
       </c>
       <c r="C2">
-        <v>0.59750000000000003</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,13 +464,13 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B3">
-        <v>309</v>
+        <v>158</v>
       </c>
       <c r="C3">
-        <v>0.77249999999999996</v>
+        <v>0.79</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,13 +478,13 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B4">
-        <v>315</v>
+        <v>197</v>
       </c>
       <c r="C4">
-        <v>0.78749999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,13 +492,13 @@
         <v>0.375</v>
       </c>
       <c r="B5">
-        <v>443</v>
+        <v>251</v>
       </c>
       <c r="C5">
-        <v>0.73833333333333329</v>
+        <v>0.62749999999999995</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B6">
-        <v>454</v>
+        <v>302</v>
       </c>
       <c r="C6">
-        <v>0.75666666666666671</v>
+        <v>0.755</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,13 +520,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B7">
-        <v>547</v>
+        <v>331</v>
       </c>
       <c r="C7">
-        <v>0.91166666666666663</v>
+        <v>0.82750000000000001</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,13 +534,13 @@
         <v>0.5</v>
       </c>
       <c r="B8">
-        <v>613</v>
+        <v>253</v>
       </c>
       <c r="C8">
-        <v>0.76624999999999999</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,13 +548,13 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B9">
-        <v>582</v>
+        <v>264</v>
       </c>
       <c r="C9">
-        <v>0.97</v>
+        <v>0.66</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,13 +562,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B10">
-        <v>568</v>
+        <v>268</v>
       </c>
       <c r="C10">
-        <v>0.94666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,13 +576,13 @@
         <v>0.625</v>
       </c>
       <c r="B11">
-        <v>639</v>
+        <v>278</v>
       </c>
       <c r="C11">
-        <v>0.79874999999999996</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,13 +590,13 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B12">
-        <v>670</v>
+        <v>261</v>
       </c>
       <c r="C12">
-        <v>0.83750000000000002</v>
+        <v>0.65249999999999997</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,13 +604,13 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B13">
-        <v>584</v>
+        <v>266</v>
       </c>
       <c r="C13">
-        <v>0.97333333333333338</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,13 +618,13 @@
         <v>0.75</v>
       </c>
       <c r="B14">
-        <v>467</v>
+        <v>181</v>
       </c>
       <c r="C14">
-        <v>0.77833333333333332</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,13 +632,13 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B15">
-        <v>336</v>
+        <v>154</v>
       </c>
       <c r="C15">
-        <v>0.84</v>
+        <v>0.77</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,13 +646,13 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B16">
-        <v>233</v>
+        <v>100</v>
       </c>
       <c r="C16">
-        <v>0.58250000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,10 +660,10 @@
         <v>0.875</v>
       </c>
       <c r="B17">
-        <v>192</v>
+        <v>75</v>
       </c>
       <c r="C17">
-        <v>0.96</v>
+        <v>0.375</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -674,10 +674,10 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B18">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="C18">
-        <v>0.71499999999999997</v>
+        <v>0.18</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -688,10 +688,10 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B19">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C19">
-        <v>0.40500000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -702,10 +702,10 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C20">
-        <v>0.44500000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -716,10 +716,10 @@
         <v>1.0416666666666701</v>
       </c>
       <c r="B21">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C21">
-        <v>0.39</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -730,10 +730,10 @@
         <v>1.0833333333333299</v>
       </c>
       <c r="B22">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>0.375</v>
+        <v>0.185</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -744,10 +744,10 @@
         <v>1.125</v>
       </c>
       <c r="B23">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>0.34499999999999997</v>
+        <v>0.105</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>1.1666666666666701</v>
       </c>
       <c r="B24">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="C24">
-        <v>0.63</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -772,10 +772,10 @@
         <v>1.2083333333333299</v>
       </c>
       <c r="B25">
-        <v>177</v>
+        <v>77</v>
       </c>
       <c r="C25">
-        <v>0.88500000000000001</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="D25">
         <v>1</v>

</xml_diff>